<commit_message>
Aktivitätsdiagramm & Boxes Excel
</commit_message>
<xml_diff>
--- a/Boxes/Boxes.xlsx
+++ b/Boxes/Boxes.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D162" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O204" sqref="O204"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1891,7 +1891,7 @@
         <v>61</v>
       </c>
       <c r="C116" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
@@ -2417,6 +2417,9 @@
       <c r="B168" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C168" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
@@ -2462,6 +2465,9 @@
       </c>
       <c r="B173" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="C173" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>